<commit_message>
Dynamic changing of while temperature condition
</commit_message>
<xml_diff>
--- a/Time_Cost-Analysis/Data_Analyze_SA.xlsx
+++ b/Time_Cost-Analysis/Data_Analyze_SA.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sw008\OneDrive - 중앙대학교\과제\인공지능\TSP-improving\Time_Cost-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="382" documentId="8_{CA113595-315F-4677-9847-C90791452CA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1783D900-9242-4218-93BD-75D14CAAD1CB}"/>
+  <xr:revisionPtr revIDLastSave="467" documentId="8_{CA113595-315F-4677-9847-C90791452CA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B65D4969-67E2-4D31-B466-3D2FA2B05BB4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{E3CB97A0-1B56-4550-824D-6942D65F0376}"/>
+    <workbookView xWindow="25380" yWindow="1776" windowWidth="30960" windowHeight="12204" xr2:uid="{E3CB97A0-1B56-4550-824D-6942D65F0376}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$P$26:$P$29</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$Q$26:$Q$29</definedName>
+  </definedNames>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>Time</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -86,12 +90,16 @@
     <t>Propriate while temp</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">Final </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,8 +141,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +170,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -211,7 +232,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -224,8 +245,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -238,11 +262,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="계산" xfId="1" builtinId="22"/>
     <cellStyle name="메모" xfId="3" builtinId="10"/>
     <cellStyle name="셀 확인" xfId="2" builtinId="23"/>
+    <cellStyle name="좋음" xfId="4" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -273,6 +301,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>cost per While condition </a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -726,6 +780,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1618902912"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -797,75 +852,9 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
-              <a:t>% of Cost</a:t>
-            </a:r>
-            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ko-KR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.2055888258532489E-2"/>
-          <c:y val="0.20770784368272485"/>
-          <c:w val="0.85196910557493744"/>
-          <c:h val="0.74634925791366424"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -900,87 +889,13 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:forward val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:forward val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1016,17 +931,20 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$26:$P$28</c:f>
+              <c:f>Sheet1!$P$26:$P$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>131</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1083</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1599</c:v>
                 </c:pt>
               </c:numCache>
@@ -1034,17 +952,20 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$26:$Q$28</c:f>
+              <c:f>Sheet1!$Q$26:$Q$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1300</c:v>
                 </c:pt>
               </c:numCache>
@@ -1053,7 +974,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7CEA-495A-A74D-BB440AB3643D}"/>
+              <c16:uniqueId val="{00000000-5A85-4D20-B5FF-BFC9653BF6D7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1065,11 +986,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1717529920"/>
-        <c:axId val="1381360624"/>
+        <c:axId val="1779374496"/>
+        <c:axId val="1569510400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1717529920"/>
+        <c:axId val="1779374496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1112,12 +1033,12 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1381360624"/>
+        <c:crossAx val="1569510400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1381360624"/>
+        <c:axId val="1569510400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,7 +1089,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1717529920"/>
+        <c:crossAx val="1779374496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1808,7 +1729,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1916,6 +1837,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1926,6 +1852,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1957,6 +1888,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2350,23 +2284,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>612065</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>212463</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>441414</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>159416</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>1038785</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>79786</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1176909</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>60024</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="차트 3">
+        <xdr:cNvPr id="3" name="차트 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85993DBF-D632-4394-A2B3-3D0DF19A780C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480BD439-1289-4FEC-A212-7DEC82CBC286}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2684,10 +2618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8E92C9-2643-46B3-99C3-199ADCAFD7C0}">
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3505,46 +3439,96 @@
         <v>0.97649076270855195</v>
       </c>
     </row>
-    <row r="19" spans="5:25" x14ac:dyDescent="0.4">
-      <c r="E19" s="3">
-        <f>AVERAGE(E3:E18)</f>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="E14" s="3">
+        <f ca="1">AVERAGE(E3:E18)</f>
         <v>5.3855342600080665</v>
       </c>
-      <c r="F19" s="3">
-        <f t="shared" ref="F19:G19" si="3">AVERAGE(F3:F18)</f>
+      <c r="F14" s="3">
+        <f ca="1">AVERAGE(F3:F18)</f>
         <v>608.23147937112014</v>
       </c>
-      <c r="G19" s="3">
-        <f t="shared" si="3"/>
+      <c r="G14" s="3">
+        <f ca="1">AVERAGE(G3:G18)</f>
         <v>46.333333333333336</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="N19" s="3">
-        <f>AVERAGE(N3:N18)</f>
+      <c r="H14" s="3"/>
+      <c r="N14" s="3">
+        <f ca="1">AVERAGE(N3:N18)</f>
         <v>24.690518405702335</v>
       </c>
-      <c r="O19" s="3">
-        <f t="shared" ref="O19" si="4">AVERAGE(O3:O18)</f>
+      <c r="O14" s="3">
+        <f ca="1">AVERAGE(O3:O18)</f>
         <v>4719.6068009385535</v>
       </c>
-      <c r="P19" s="3">
-        <f t="shared" ref="P19" si="5">AVERAGE(P3:P18)</f>
+      <c r="P14" s="3">
+        <f ca="1">AVERAGE(P3:P18)</f>
         <v>42.555555555555557</v>
       </c>
-      <c r="W19" s="3">
-        <f>AVERAGE(W3:W18)</f>
+      <c r="W14" s="3">
+        <f ca="1">AVERAGE(W3:W18)</f>
         <v>30.647693845960777</v>
       </c>
-      <c r="X19" s="3">
-        <f t="shared" ref="X19" si="6">AVERAGE(X3:X18)</f>
+      <c r="X14" s="3">
+        <f ca="1">AVERAGE(X3:X18)</f>
         <v>7040.7734732134059</v>
       </c>
-      <c r="Y19" s="3">
-        <f t="shared" ref="Y19" si="7">AVERAGE(Y3:Y18)</f>
+      <c r="Y14" s="3">
+        <f ca="1">AVERAGE(Y3:Y18)</f>
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="5:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="4:26" x14ac:dyDescent="0.4">
+      <c r="D19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="4">
+        <v>6.5425302982330296</v>
+      </c>
+      <c r="F19" s="4">
+        <v>598.26079339348098</v>
+      </c>
+      <c r="G19" s="4">
+        <v>56</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" ref="H19" si="3">F19/$F$3</f>
+        <v>1.0001170192189215</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N19" s="4">
+        <v>13.9063436985015</v>
+      </c>
+      <c r="O19" s="4">
+        <v>4692.4896430914096</v>
+      </c>
+      <c r="P19" s="4">
+        <v>23</v>
+      </c>
+      <c r="Q19" s="4">
+        <f t="shared" ref="Q19" si="4">O19/$O$3</f>
+        <v>0.98199799880690031</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W19" s="4">
+        <v>13.6781260967254</v>
+      </c>
+      <c r="X19" s="4">
+        <v>6984.0578117752602</v>
+      </c>
+      <c r="Y19" s="4">
+        <v>20</v>
+      </c>
+      <c r="Z19" s="4">
+        <f t="shared" ref="Z19" si="5">X19/$O$3</f>
+        <v>1.4615548070121558</v>
+      </c>
+    </row>
+    <row r="25" spans="4:26" x14ac:dyDescent="0.4">
       <c r="P25" t="s">
         <v>11</v>
       </c>
@@ -3552,31 +3536,42 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="5:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="4:26" x14ac:dyDescent="0.4">
       <c r="P26">
-        <v>131</v>
+        <v>50</v>
       </c>
       <c r="Q26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="5:25" x14ac:dyDescent="0.4">
+    <row r="27" spans="4:26" x14ac:dyDescent="0.4">
       <c r="P27">
+        <v>131</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="4:26" x14ac:dyDescent="0.4">
+      <c r="P28">
         <v>1083</v>
       </c>
-      <c r="Q27">
+      <c r="Q28">
         <v>800</v>
       </c>
     </row>
-    <row r="28" spans="5:25" x14ac:dyDescent="0.4">
-      <c r="P28">
+    <row r="29" spans="4:26" x14ac:dyDescent="0.4">
+      <c r="P29">
         <v>1599</v>
       </c>
-      <c r="Q28">
+      <c r="Q29">
         <v>1300</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P26:Q29">
+    <sortCondition ref="P26"/>
+  </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3585,6 +3580,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x010100D94E01AD38B9A7499D640DDC9AABD88F" ma:contentTypeVersion="10" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="03a66fc9afa39527380bd317f6aa3292">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e853eb9a-ebd3-4eed-8cb6-8c1751577767" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="574bf45a50b0194fbac0600a3b6efe76" ns3:_="">
     <xsd:import namespace="e853eb9a-ebd3-4eed-8cb6-8c1751577767"/>
@@ -3768,22 +3778,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55579AE9-22FD-4D29-A109-4AB051F3639C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAE3478E-6FD3-48B5-A71D-89B7B7BF878A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59CB7ECB-F669-4B54-9E67-C2E0067E23D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3799,21 +3811,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAE3478E-6FD3-48B5-A71D-89B7B7BF878A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55579AE9-22FD-4D29-A109-4AB051F3639C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>